<commit_message>
chore: update music spreadsheet
</commit_message>
<xml_diff>
--- a/src/Music.xlsx
+++ b/src/Music.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="404">
   <si>
     <t>Song Name</t>
   </si>
@@ -25,6 +25,18 @@
     <t>Playlist</t>
   </si>
   <si>
+    <t>Take Me Away</t>
+  </si>
+  <si>
+    <t>ACRAZE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Wn58vqKvAQA</t>
+  </si>
+  <si>
+    <t>TECH HOUSE</t>
+  </si>
+  <si>
     <t>Dame mas Gasolina</t>
   </si>
   <si>
@@ -64,6 +76,15 @@
     <t>https://www.youtube.com/watch?v=ViAWRL9Jw4c</t>
   </si>
   <si>
+    <t>Friday (Alone Right Now)</t>
+  </si>
+  <si>
+    <t>ATRIP</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=MFTFRW69PCM</t>
+  </si>
+  <si>
     <t>Wacuka</t>
   </si>
   <si>
@@ -73,36 +94,33 @@
     <t>https://www.youtube.com/watch?v=15bxsb7VrZs</t>
   </si>
   <si>
+    <t>All We Need</t>
+  </si>
+  <si>
+    <t>AYYBO</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=8xa4ihnyII8</t>
+  </si>
+  <si>
+    <t>Certified</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=FjebtlbhnO8</t>
+  </si>
+  <si>
+    <t>Demon Time</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=pyuiZwxIGCQ</t>
+  </si>
+  <si>
     <t>Rizz</t>
   </si>
   <si>
-    <t>AYYBO</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=yJvfvVmE81c</t>
   </si>
   <si>
-    <t>TECH HOUSE</t>
-  </si>
-  <si>
-    <t>Demon Time</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=pyuiZwxIGCQ</t>
-  </si>
-  <si>
-    <t>All We Need</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=8xa4ihnyII8</t>
-  </si>
-  <si>
-    <t>Certified</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=FjebtlbhnO8</t>
-  </si>
-  <si>
     <t>Glue</t>
   </si>
   <si>
@@ -112,19 +130,37 @@
     <t>https://www.youtube.com/watch?v=A7ZxRs45tTg</t>
   </si>
   <si>
+    <t>Ballo</t>
+  </si>
+  <si>
+    <t>BISCITS</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=iE2z8-2qYio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't stop </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=iJLXvd0sg50</t>
+  </si>
+  <si>
     <t>Freak (GREG Remix)</t>
   </si>
   <si>
-    <t>BISCITS</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=oxJPLTEyTU4</t>
   </si>
   <si>
-    <t xml:space="preserve">Don't stop </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=iJLXvd0sg50</t>
+    <t>I am the One</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lZHA9Rrx8aI</t>
+  </si>
+  <si>
+    <t>In the Place</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=m_2cQPflGLs</t>
   </si>
   <si>
     <t>Jungle</t>
@@ -133,36 +169,27 @@
     <t>https://www.youtube.com/watch?v=DjtThvFuLWY</t>
   </si>
   <si>
-    <t>In the Place</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=m_2cQPflGLs</t>
-  </si>
-  <si>
     <t>Mantra</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=2LDwqw_Tclc</t>
   </si>
   <si>
-    <t>Ballo</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=iE2z8-2qYio</t>
-  </si>
-  <si>
-    <t>I am the One</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=lZHA9Rrx8aI</t>
-  </si>
-  <si>
     <t>Tribalism</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=H8CHNfmi9rw</t>
   </si>
   <si>
+    <t xml:space="preserve">Despacio </t>
+  </si>
+  <si>
+    <t>Bontan</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=TH3r5PJOciQ</t>
+  </si>
+  <si>
     <t xml:space="preserve">how deep is your love </t>
   </si>
   <si>
@@ -190,39 +217,39 @@
     <t>https://www.youtube.com/watch?v=BxXSGL1iC_w</t>
   </si>
   <si>
+    <t>beggin'</t>
+  </si>
+  <si>
+    <t>Chris Lake</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ckvSfTFCqUk</t>
+  </si>
+  <si>
+    <t>ease my mind</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9DOADMsS7mk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in the yuma </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=OOIjkdUZKRs</t>
+  </si>
+  <si>
+    <t>more baby</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6ooxackHbY4</t>
+  </si>
+  <si>
     <t>percolator</t>
   </si>
   <si>
-    <t>Chris Lake</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=16vVRMQqa2I</t>
   </si>
   <si>
-    <t xml:space="preserve">in the yuma </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=OOIjkdUZKRs</t>
-  </si>
-  <si>
-    <t>beggin'</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=ckvSfTFCqUk</t>
-  </si>
-  <si>
-    <t>more baby</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=6ooxackHbY4</t>
-  </si>
-  <si>
-    <t>ease my mind</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=9DOADMsS7mk</t>
-  </si>
-  <si>
     <t xml:space="preserve">summertime </t>
   </si>
   <si>
@@ -232,45 +259,51 @@
     <t>https://www.youtube.com/watch?v=gTdZb7l3YnM</t>
   </si>
   <si>
+    <t>california dreaming</t>
+  </si>
+  <si>
+    <t>Chris Lorenzo</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=r7u5UwWO6-4</t>
+  </si>
+  <si>
+    <t>pump</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=K7P5ftpMvls</t>
+  </si>
+  <si>
     <t xml:space="preserve">u should not be doing that </t>
   </si>
   <si>
-    <t>Chris Lorenzo</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=9sQtfM9oPs0</t>
   </si>
   <si>
-    <t>pump</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=K7P5ftpMvls</t>
-  </si>
-  <si>
-    <t>california dreaming</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=r7u5UwWO6-4</t>
+    <t>MAMI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qQqL7Rbpo0o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desire </t>
+  </si>
+  <si>
+    <t>Chris Stussy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wt9rHax4ciY</t>
   </si>
   <si>
     <t xml:space="preserve">seeing and believeing </t>
   </si>
   <si>
-    <t>Chris Stussy</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=oMsBdXH0jts</t>
   </si>
   <si>
     <t>HOUSE</t>
   </si>
   <si>
-    <t xml:space="preserve">desire </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=wt9rHax4ciY</t>
-  </si>
-  <si>
     <t>The Days (Notion Remix)</t>
   </si>
   <si>
@@ -280,64 +313,67 @@
     <t>https://www.youtube.com/watch?v=RUm36FWCyqA</t>
   </si>
   <si>
+    <t xml:space="preserve">Fine Night </t>
+  </si>
+  <si>
+    <t>CLOONEE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=0cc-Li6B9EU</t>
+  </si>
+  <si>
+    <t>Get Stupid</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=V9cG9ZYccMY</t>
+  </si>
+  <si>
+    <t>Love You Like That</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=JJOxxbAP6FI</t>
+  </si>
+  <si>
     <t>Mi Amor</t>
   </si>
   <si>
-    <t>CLOONEE</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=6-8z05nMFv4</t>
   </si>
   <si>
+    <t>Pegao</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GxrNnrCmI1s</t>
+  </si>
+  <si>
+    <t>Stephanie</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=stlEtYDr27M</t>
+  </si>
+  <si>
+    <t>To The Beat</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=05q2XvPSgv0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to the beat </t>
+  </si>
+  <si>
     <t>Tripasia</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=tcmiiZLJQ4c</t>
   </si>
   <si>
-    <t>Get Stupid</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=V9cG9ZYccMY</t>
-  </si>
-  <si>
-    <t>Love You Like That</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=JJOxxbAP6FI</t>
-  </si>
-  <si>
-    <t>To The Beat</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=05q2XvPSgv0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fine Night </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=0cc-Li6B9EU</t>
-  </si>
-  <si>
-    <t>Stephanie</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=stlEtYDr27M</t>
-  </si>
-  <si>
     <t>Still my baby</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=I-XG_z-25i4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to the beat </t>
-  </si>
-  <si>
-    <t>Pegao</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=GxrNnrCmI1s</t>
+    <t>CLOONEE &amp; GREG (BR)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2wU6MW0kcew</t>
   </si>
   <si>
     <t xml:space="preserve">super sonic </t>
@@ -358,6 +394,24 @@
     <t>https://www.youtube.com/watch?v=tAMY6KNhw_8</t>
   </si>
   <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Dave Winnel</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lvqOcjZrXxA</t>
+  </si>
+  <si>
+    <t>I Remember (John Summit)</t>
+  </si>
+  <si>
+    <t>deadmau5 &amp; Kaskade</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=UV8a-NmM2Zc</t>
+  </si>
+  <si>
     <t xml:space="preserve">your love </t>
   </si>
   <si>
@@ -367,6 +421,15 @@
     <t>https://www.youtube.com/watch?v=1rJS9MZaXgA</t>
   </si>
   <si>
+    <t>Stay High</t>
+  </si>
+  <si>
+    <t>Diplo &amp; HUGEL</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lrNnkB1skGc</t>
+  </si>
+  <si>
     <t xml:space="preserve">when a fire starts to burn akapella </t>
   </si>
   <si>
@@ -385,21 +448,21 @@
     <t>Disco Lines</t>
   </si>
   <si>
+    <t xml:space="preserve">disco boy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disco Lines </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=t1RBTk8liE8</t>
+  </si>
+  <si>
     <t>kiss - i was made for loving you</t>
   </si>
   <si>
-    <t xml:space="preserve">Disco Lines </t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=ETMMkMDSDLo</t>
   </si>
   <si>
-    <t xml:space="preserve">disco boy </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=t1RBTk8liE8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sexy Ass Trumpets </t>
   </si>
   <si>
@@ -448,6 +511,21 @@
     <t>https://www.youtube.com/watch?v=QqdN3p50Q4U</t>
   </si>
   <si>
+    <t>Miracle Maker</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=e7HyuhQPMy4</t>
+  </si>
+  <si>
+    <t>Eat your Man</t>
+  </si>
+  <si>
+    <t>Dom Dolla &amp; Nelly Furtado</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=bqAvZ4Y7kGI</t>
+  </si>
+  <si>
     <t>Nokia</t>
   </si>
   <si>
@@ -460,85 +538,118 @@
     <t>ELECTRO POP</t>
   </si>
   <si>
+    <t>atmosphere</t>
+  </si>
+  <si>
+    <t>Fisher</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1Y1g-J751lE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boost Up </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=g5m92mXtUYs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">its that time </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=3Ioi8qE8afY</t>
+  </si>
+  <si>
+    <t>jamming</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7p2Lzw23Upo</t>
+  </si>
+  <si>
+    <t>ocean</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=AdbMlNNORJE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">somebody </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QCekLn0YIaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">world hold on </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Qf1Dv2ZMudE</t>
+  </si>
+  <si>
     <t xml:space="preserve">yeah the girls </t>
   </si>
   <si>
-    <t>Fisher</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=poH1lqLgZAc</t>
   </si>
   <si>
-    <t>atmosphere</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=1Y1g-J751lE</t>
-  </si>
-  <si>
-    <t>ocean</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=AdbMlNNORJE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">its that time </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=3Ioi8qE8afY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boost Up </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=g5m92mXtUYs</t>
-  </si>
-  <si>
-    <t>jamming</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=7p2Lzw23Upo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">world hold on </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=Qf1Dv2ZMudE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">somebody </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=QCekLn0YIaw</t>
+    <t>It's A Killa</t>
+  </si>
+  <si>
+    <t>Fisher &amp; Shermanology</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=P8qwTPNTY9Q</t>
+  </si>
+  <si>
+    <t>Adore u</t>
+  </si>
+  <si>
+    <t>Fred Again</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=jJ6LjK1yDRs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">danielle </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qJ1GBL1TPLg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delilah </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Cl6Rz1Uvi2M</t>
   </si>
   <si>
     <t>jungle</t>
   </si>
   <si>
-    <t>Fred Again</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=dba_lEJGXf4</t>
   </si>
   <si>
-    <t xml:space="preserve">delilah </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=Cl6Rz1Uvi2M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">danielle </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=qJ1GBL1TPLg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alone right now </t>
-  </si>
-  <si>
-    <t xml:space="preserve">friday </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=MFTFRW69PCM</t>
+    <t>Stayinit</t>
+  </si>
+  <si>
+    <t>Fred Again &amp; Lil Yachty</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=K5gqOzfzBKg</t>
+  </si>
+  <si>
+    <t>Strong</t>
+  </si>
+  <si>
+    <t>Fred Again &amp; Romy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Koju3Qk2bVk</t>
+  </si>
+  <si>
+    <t>Turn on the Lights</t>
+  </si>
+  <si>
+    <t>Fred Again &amp; Swedish House Mafia</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nu8T_NBI9Bs</t>
   </si>
   <si>
     <t xml:space="preserve">freed from desire </t>
@@ -565,33 +676,33 @@
     <t>https://www.youtube.com/watch?v=Hrph2EW9VjY</t>
   </si>
   <si>
+    <t>All Good Things</t>
+  </si>
+  <si>
+    <t>Gravagerz</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=k8seB5iJGbE</t>
+  </si>
+  <si>
     <t>Chihiro</t>
   </si>
   <si>
-    <t>Gravagerz</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=eJPS5gHESCA</t>
   </si>
   <si>
+    <t>Greenlight</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_xUJut7C1t4</t>
+  </si>
+  <si>
     <t>Help Me Lose My Mind</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=lBuoLcogx8k</t>
   </si>
   <si>
-    <t>All Good Things</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=k8seB5iJGbE</t>
-  </si>
-  <si>
-    <t>Greenlight</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=_xUJut7C1t4</t>
-  </si>
-  <si>
     <t>Whispers</t>
   </si>
   <si>
@@ -658,19 +769,25 @@
     <t>https://www.youtube.com/watch?v=JOfdYKGVnzA</t>
   </si>
   <si>
+    <t>escape</t>
+  </si>
+  <si>
+    <t>John Summit</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=P6LSIBpCzrc</t>
+  </si>
+  <si>
     <t>Go Back (Kyle Watson Remix)</t>
   </si>
   <si>
-    <t>John Summit</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=dAWUwcGx83s</t>
   </si>
   <si>
-    <t>escape</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=P6LSIBpCzrc</t>
+    <t xml:space="preserve">make me feel </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=BpK4reYkfUg</t>
   </si>
   <si>
     <t>palm of my hands</t>
@@ -685,22 +802,28 @@
     <t>https://www.youtube.com/watch?v=hHsUT3INgsI</t>
   </si>
   <si>
+    <t>Sweet Disposition</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=WStAm_BrkGI</t>
+  </si>
+  <si>
+    <t>tears</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kPQaB0nZiwc</t>
+  </si>
+  <si>
     <t xml:space="preserve">where you are </t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=i6vmJNnPtwQ</t>
   </si>
   <si>
-    <t>tears</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=kPQaB0nZiwc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make me feel </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=BpK4reYkfUg</t>
+    <t>Legacy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=eOnv8Nu85jU</t>
   </si>
   <si>
     <t>luther</t>
@@ -712,6 +835,12 @@
     <t>https://www.youtube.com/watch?v=GS9uNbSwMHs</t>
   </si>
   <si>
+    <t>Not Like Us (Sam Collin &amp; Sly Phil)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LcwRQaaAE8M</t>
+  </si>
+  <si>
     <t>Thandaza</t>
   </si>
   <si>
@@ -730,21 +859,21 @@
     <t>https://www.youtube.com/watch?v=MOenJHdj8ro</t>
   </si>
   <si>
+    <t>Messy (Laszewo Edit)</t>
+  </si>
+  <si>
+    <t>Laszewo</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=AcYGpEqITKs</t>
+  </si>
+  <si>
     <t>Sailor Song (Laszewo Edit)</t>
   </si>
   <si>
-    <t>Laszewo</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=RYd_rBgRkmM</t>
   </si>
   <si>
-    <t>Messy (Laszewo Edit)</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=AcYGpEqITKs</t>
-  </si>
-  <si>
     <t>Meet me in the middle</t>
   </si>
   <si>
@@ -754,6 +883,15 @@
     <t>https://www.youtube.com/watch?v=OFnKV8rk96E</t>
   </si>
   <si>
+    <t>Last Night</t>
+  </si>
+  <si>
+    <t>Loofy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fHZRijtV4Q0</t>
+  </si>
+  <si>
     <t xml:space="preserve">When I Close My Eyes </t>
   </si>
   <si>
@@ -763,6 +901,15 @@
     <t>https://www.youtube.com/watch?v=p0beTMamdZM</t>
   </si>
   <si>
+    <t>Can't Fight the Feeling</t>
+  </si>
+  <si>
+    <t>Matroda</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=yXAwr-EfpJQ</t>
+  </si>
+  <si>
     <t xml:space="preserve">it feels so god </t>
   </si>
   <si>
@@ -787,6 +934,24 @@
     <t>https://www.youtube.com/watch?v=8jKT_kr-7eU</t>
   </si>
   <si>
+    <t>Dress Code</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=L3VTqqbKc_w&amp;</t>
+  </si>
+  <si>
+    <t>Drugs from Amsterdam</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4_pnZ5ixYWU</t>
+  </si>
+  <si>
+    <t>Beats for the Underground</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4x91fxE0NWQ</t>
+  </si>
+  <si>
     <t>Slow Down (Vintage Culture Remix)</t>
   </si>
   <si>
@@ -805,6 +970,12 @@
     <t>https://www.youtube.com/watch?v=6gq-MlQGkOY</t>
   </si>
   <si>
+    <t>Jealous</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LOEIJ3KO2HM</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAY MY NAME </t>
   </si>
   <si>
@@ -832,6 +1003,15 @@
     <t>https://www.youtube.com/watch?v=8Nn3uUrEUCQ</t>
   </si>
   <si>
+    <t>Burnin'</t>
+  </si>
+  <si>
+    <t>Noizu</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XgfF6L0VHNI</t>
+  </si>
+  <si>
     <t xml:space="preserve">blackwater </t>
   </si>
   <si>
@@ -841,6 +1021,15 @@
     <t>https://www.youtube.com/watch?v=M0b5D2NC0zE</t>
   </si>
   <si>
+    <t>Losing Control</t>
+  </si>
+  <si>
+    <t>Odd Mob</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Mg1QHSrkRx0</t>
+  </si>
+  <si>
     <t xml:space="preserve">i was made for lovin you </t>
   </si>
   <si>
@@ -850,33 +1039,42 @@
     <t>https://www.youtube.com/watch?v=hH_HpuE6lE4</t>
   </si>
   <si>
+    <t>Devon (Oliver Huntemann Remix)</t>
+  </si>
+  <si>
+    <t>Oliver Schories</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZAq5OyuLDQA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dirty cash </t>
+  </si>
+  <si>
+    <t>PAWSA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fIHTdO96a60</t>
+  </si>
+  <si>
+    <t>ON THE MOVE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4pM0TPBs2bU</t>
+  </si>
+  <si>
+    <t>PICK UP THE PHONE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Ko1QI6ZkUFE</t>
+  </si>
+  <si>
     <t>TOO COOL TO BE CARELESS</t>
   </si>
   <si>
-    <t>PAWSA</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=Mo1uf9cAJxM</t>
   </si>
   <si>
-    <t>PICK UP THE PHONE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=Ko1QI6ZkUFE</t>
-  </si>
-  <si>
-    <t>ON THE MOVE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=4pM0TPBs2bU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dirty cash </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=fIHTdO96a60</t>
-  </si>
-  <si>
     <t xml:space="preserve">this rhythm </t>
   </si>
   <si>
@@ -940,33 +1138,39 @@
     <t>https://www.youtube.com/watch?v=gAthBqFxi50</t>
   </si>
   <si>
+    <t>Beat of the Drum</t>
+  </si>
+  <si>
+    <t>Shermanology</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=NdAW695I2VU</t>
+  </si>
+  <si>
+    <t>boys n da club</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fMxR0HTvu3U</t>
+  </si>
+  <si>
     <t>ready 2 go</t>
   </si>
   <si>
-    <t>Shermanology</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=zrkbYyasIW8</t>
   </si>
   <si>
-    <t>boys n da club</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=fMxR0HTvu3U</t>
-  </si>
-  <si>
-    <t>Beat of the Drum</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=NdAW695I2VU</t>
+    <t>Don't Keep Me Waiting</t>
+  </si>
+  <si>
+    <t>Sidepiece</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=8ws62tljIn8</t>
   </si>
   <si>
     <t xml:space="preserve">menege a trois </t>
   </si>
   <si>
-    <t>Sidepiece</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=-cy5D6FORlU</t>
   </si>
   <si>
@@ -976,10 +1180,13 @@
     <t>https://www.youtube.com/watch?v=wuVssXgHH8Q</t>
   </si>
   <si>
-    <t>Don't Keep Me Waiting</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=8ws62tljIn8</t>
+    <t>Rumble</t>
+  </si>
+  <si>
+    <t>Skrillex &amp; Fred Again</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kP2ky9l43dg</t>
   </si>
   <si>
     <t>tell me</t>
@@ -991,53 +1198,38 @@
     <t>https://www.youtube.com/watch?v=t5EDvlzQfzw</t>
   </si>
   <si>
-    <t xml:space="preserve">despacio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">unknown </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=TH3r5PJOciQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cool lil instrumental </t>
-  </si>
-  <si>
-    <t xml:space="preserve">who the fuck knows </t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=ZAq5OyuLDQA</t>
-  </si>
-  <si>
-    <t>Rumble</t>
-  </si>
-  <si>
-    <t>Skrillex &amp; Fred Again</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=kP2ky9l43dg</t>
-  </si>
-  <si>
-    <t>Stayinit</t>
-  </si>
-  <si>
-    <t>Fred Again &amp; Lil Yachty</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=K5gqOzfzBKg</t>
-  </si>
-  <si>
-    <t>Adore u</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=jJ6LjK1yDRs</t>
+    <t>Blow (White Girl in Town)</t>
+  </si>
+  <si>
+    <t>Sosa UK</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wJZQDRfoBIU</t>
+  </si>
+  <si>
+    <t>Buscando Money</t>
+  </si>
+  <si>
+    <t>Twenty Six</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sxNxlcS8f4w</t>
+  </si>
+  <si>
+    <t>You Give Me A Feeling</t>
+  </si>
+  <si>
+    <t>Vintage Culture &amp; James Hype</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ABAlIBtd_Ew</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1055,7 +1247,7 @@
     </font>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF434343"/>
       <name val="Roboto"/>
     </font>
     <font>
@@ -1080,7 +1272,12 @@
     </font>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF434343"/>
       <name val="Roboto"/>
     </font>
     <font>
@@ -1090,7 +1287,17 @@
     </font>
     <font>
       <u/>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
       <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF434343"/>
       <name val="Roboto"/>
     </font>
   </fonts>
@@ -1276,7 +1483,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1313,31 +1520,58 @@
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="8" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1346,7 +1580,7 @@
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1410,7 +1644,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D132" displayName="Music" name="Music" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D156" displayName="Music" name="Music" id="1">
   <tableColumns count="4">
     <tableColumn name="Song Name" id="1"/>
     <tableColumn name="Artist" id="2"/>
@@ -1673,21 +1907,21 @@
         <v>10</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -1695,111 +1929,111 @@
         <v>15</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="12" t="s">
+      <c r="C6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="13" t="s">
         <v>22</v>
       </c>
+      <c r="C7" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="D7" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>23</v>
+      <c r="C8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>23</v>
+      <c r="C10" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>23</v>
+      <c r="D12" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -1807,139 +2041,139 @@
         <v>36</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="A14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>23</v>
+      <c r="B14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>41</v>
+      <c r="C15" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>34</v>
+      <c r="A16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>23</v>
+      <c r="A18" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>49</v>
+        <v>40</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="14" t="s">
+      <c r="A20" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>23</v>
+      <c r="B20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="18" t="s">
         <v>55</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>23</v>
+      <c r="D22" s="15" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23">
@@ -1949,893 +2183,891 @@
       <c r="B23" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="18" t="s">
         <v>61</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>23</v>
+      <c r="C24" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>23</v>
+      <c r="A26" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C27" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>23</v>
+      <c r="C28" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>74</v>
+      <c r="A30" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>23</v>
+        <v>78</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" s="6" t="s">
+      <c r="A32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="B32" s="13" t="s">
         <v>83</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>86</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="B34" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>23</v>
+      <c r="D34" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="D35" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="4" t="s">
+      <c r="B36" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>23</v>
+      <c r="D36" s="15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="23" t="s">
         <v>94</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="6" t="s">
+      <c r="A38" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>23</v>
+      <c r="B38" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="6" t="s">
+      <c r="A40" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>23</v>
+      <c r="C40" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>90</v>
+      <c r="A42" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>23</v>
+        <v>108</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="8" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>90</v>
+      <c r="A44" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D44" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>111</v>
+        <v>101</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C46" s="14" t="s">
+      <c r="A46" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>23</v>
+      <c r="D46" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C47" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="10" t="s">
         <v>117</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>121</v>
+      <c r="D48" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="C49" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C49" s="13" t="s">
-        <v>75</v>
-      </c>
       <c r="D49" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>23</v>
+      <c r="D50" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C51" s="10" t="s">
+      <c r="B51" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="D51" s="11" t="s">
-        <v>23</v>
+      <c r="C51" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>23</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52" s="7"/>
     </row>
     <row r="53">
       <c r="A53" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>75</v>
+        <v>134</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="4" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>75</v>
+        <v>137</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>137</v>
+      <c r="A55" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>141</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>23</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>23</v>
+      <c r="A56" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="8" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>23</v>
+      <c r="A58" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="8" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C59" s="13" t="s">
-        <v>147</v>
+      <c r="C59" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>148</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>23</v>
+      <c r="A60" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="8" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>23</v>
+      <c r="A62" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="8" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>23</v>
+      <c r="A64" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B65" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B65" s="9" t="s">
-        <v>150</v>
-      </c>
       <c r="C65" s="10" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>150</v>
+        <v>166</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>160</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>23</v>
+      <c r="A67" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>23</v>
+      <c r="A68" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="8" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>14</v>
+      <c r="A70" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="8" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B72" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>177</v>
-      </c>
       <c r="C72" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>23</v>
+        <v>183</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="8" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>75</v>
+        <v>176</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>185</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>182</v>
+      <c r="A74" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>176</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>121</v>
+        <v>187</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="8" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>14</v>
+      <c r="A76" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>14</v>
+      <c r="A77" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="C77" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D77" s="22" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C78" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>14</v>
+      <c r="A78" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="8" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B80" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>197</v>
-      </c>
       <c r="C80" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>23</v>
+        <v>201</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="8" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>202</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="B82" s="5" t="s">
+      <c r="A82" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="B82" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="D82" s="7" t="s">
-        <v>23</v>
+      <c r="C82" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="B83" s="9" t="s">
+      <c r="A83" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="B83" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="D83" s="11" t="s">
-        <v>83</v>
+      <c r="C83" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="D83" s="22" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="C85" s="10" t="s">
         <v>214</v>
       </c>
+      <c r="C85" s="18" t="s">
+        <v>215</v>
+      </c>
       <c r="D85" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="B86" s="5" t="s">
+      <c r="A86" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="B86" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="D86" s="7" t="s">
-        <v>23</v>
+      <c r="C86" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="87">
@@ -2843,648 +3075,982 @@
         <v>218</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="C87" s="10" t="s">
         <v>219</v>
       </c>
+      <c r="C87" s="18" t="s">
+        <v>220</v>
+      </c>
       <c r="D87" s="11" t="s">
-        <v>23</v>
+        <v>142</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C88" s="6" t="s">
+      <c r="A88" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="D88" s="7" t="s">
-        <v>23</v>
+      <c r="B88" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B89" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="B89" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="C89" s="13" t="s">
-        <v>223</v>
+      <c r="C89" s="10" t="s">
+        <v>225</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>23</v>
+      <c r="A90" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="8" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>23</v>
+      <c r="A92" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="8" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="C93" s="19" t="s">
-        <v>232</v>
+        <v>234</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>235</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C94" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>202</v>
+      <c r="A94" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="8" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>202</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>23</v>
+      <c r="A96" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="8" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="C97" s="13" t="s">
-        <v>243</v>
+        <v>247</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>248</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="D98" s="7" t="s">
-        <v>14</v>
+      <c r="A98" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="C98" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="8" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="C99" s="10" t="s">
-        <v>249</v>
+        <v>253</v>
+      </c>
+      <c r="C99" s="28" t="s">
+        <v>254</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>251</v>
+      <c r="A100" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="B100" s="13" t="s">
+        <v>253</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>23</v>
+        <v>256</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B101" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="B101" s="9" t="s">
-        <v>254</v>
-      </c>
       <c r="C101" s="10" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>254</v>
+      <c r="A102" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>253</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="D102" s="7" t="s">
-        <v>23</v>
+        <v>260</v>
+      </c>
+      <c r="D102" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="8" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>260</v>
+        <v>253</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>262</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="C104" s="14" t="s">
-        <v>263</v>
+        <v>253</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>264</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>266</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C106" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="C106" s="6" t="s">
+      <c r="D106" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="D106" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="8" t="s">
+      <c r="B107" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C107" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="B107" s="9" t="s">
+      <c r="D107" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="C107" s="10" t="s">
+      <c r="B108" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="D107" s="11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="4" t="s">
+      <c r="C108" s="29" t="s">
         <v>273</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="D108" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="C108" s="6" t="s">
+      <c r="B109" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="C109" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="D108" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="8" t="s">
+      <c r="D109" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="B109" s="9" t="s">
+      <c r="B110" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="C109" s="13" t="s">
+      <c r="C110" s="29" t="s">
         <v>278</v>
       </c>
-      <c r="D109" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="C110" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="D110" s="7" t="s">
-        <v>23</v>
+      <c r="D110" s="15" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="8" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B111" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="C111" s="13" t="s">
+      <c r="C111" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="D111" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="B112" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="D111" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="4" t="s">
+      <c r="C112" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="B112" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="C112" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="D112" s="7" t="s">
-        <v>23</v>
+      <c r="D112" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C113" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="B113" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="C113" s="10" t="s">
+      <c r="D113" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="D113" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="4" t="s">
+      <c r="B114" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="C114" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="C114" s="6" t="s">
+      <c r="D114" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="D114" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="8" t="s">
+      <c r="B115" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="B115" s="9" t="s">
+      <c r="C115" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="C115" s="10" t="s">
+      <c r="D115" s="22"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="D115" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="4" t="s">
+      <c r="B116" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="C116" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="C116" s="6" t="s">
+      <c r="D116" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="D116" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="8" t="s">
+      <c r="B117" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="B117" s="9" t="s">
+      <c r="C117" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="C117" s="13" t="s">
+      <c r="D117" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="D117" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="4" t="s">
+      <c r="B118" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="B118" s="5" t="s">
+      <c r="C118" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="C118" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="D118" s="7" t="s">
-        <v>23</v>
+      <c r="D118" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="B119" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="B119" s="9" t="s">
+      <c r="C119" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="C119" s="13" t="s">
+      <c r="D119" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="D119" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="4" t="s">
+      <c r="B120" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C120" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="B120" s="5" t="s">
+      <c r="D120" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="C120" s="14" t="s">
+      <c r="B121" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="C121" s="21" t="s">
         <v>308</v>
       </c>
-      <c r="D120" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="B121" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="C121" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="D121" s="11" t="s">
-        <v>23</v>
+      <c r="D121" s="22" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D122" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="B123" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="C123" s="21" t="s">
         <v>312</v>
       </c>
-      <c r="B122" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="C122" s="6" t="s">
+      <c r="D123" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="D122" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="8" t="s">
+      <c r="B124" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="B123" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="C123" s="10" t="s">
+      <c r="C124" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="D123" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="D124" s="7" t="s">
-        <v>23</v>
+      <c r="D124" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B125" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C125" s="13" t="s">
-        <v>320</v>
+      <c r="C125" s="18" t="s">
+        <v>318</v>
       </c>
       <c r="D125" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>317</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D126" s="7" t="s">
-        <v>23</v>
+        <v>239</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C127" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="B127" s="9" t="s">
+      <c r="D127" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="C127" s="10" t="s">
+      <c r="B128" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="D127" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="4" t="s">
+      <c r="C128" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="B128" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="C128" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="D128" s="7" t="s">
+      <c r="D128" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="C129" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="B129" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="C129" s="13" t="s">
-        <v>331</v>
-      </c>
       <c r="D129" s="11" t="s">
-        <v>121</v>
+        <v>239</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="C130" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="B130" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>334</v>
-      </c>
       <c r="D130" s="7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="C131" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="B131" s="9" t="s">
+      <c r="D131" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="C131" s="13" t="s">
+      <c r="B132" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="D131" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="21" t="s">
+      <c r="C132" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="B132" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="C132" s="23" t="s">
+      <c r="D132" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="D132" s="24" t="s">
-        <v>23</v>
+      <c r="B133" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="C133" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="D133" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="B134" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="C134" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="D134" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C135" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="D135" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="B136" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="C136" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="D136" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C137" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="D137" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="B138" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="C138" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="D138" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C139" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="D139" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="B140" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="C140" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="D140" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="C141" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="D141" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="B142" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="C142" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="D142" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="C143" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="D143" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="B144" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="C144" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="D144" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="C145" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="D145" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="B146" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="C146" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="D146" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="C147" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="D147" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="B148" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="C148" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="D148" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="C149" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D149" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="B150" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="C150" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="D150" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="C151" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="D151" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="B152" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="C152" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="D152" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C153" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="D153" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="D154" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="B155" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="C155" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D155" s="22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="30" t="s">
+        <v>401</v>
+      </c>
+      <c r="B156" s="31" t="s">
+        <v>402</v>
+      </c>
+      <c r="C156" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="D156" s="33" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="D2:D132">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="D2:D156">
       <formula1>"LATIN HOUSE,SUNSET HOUSE,TECH HOUSE,HOUSE,DJTOOLS,ELECTRO POP,AFRO HOUSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3620,10 +4186,34 @@
     <hyperlink r:id="rId129" ref="C130"/>
     <hyperlink r:id="rId130" ref="C131"/>
     <hyperlink r:id="rId131" ref="C132"/>
+    <hyperlink r:id="rId132" ref="C133"/>
+    <hyperlink r:id="rId133" ref="C134"/>
+    <hyperlink r:id="rId134" ref="C135"/>
+    <hyperlink r:id="rId135" ref="C136"/>
+    <hyperlink r:id="rId136" ref="C137"/>
+    <hyperlink r:id="rId137" ref="C138"/>
+    <hyperlink r:id="rId138" ref="C139"/>
+    <hyperlink r:id="rId139" ref="C140"/>
+    <hyperlink r:id="rId140" ref="C141"/>
+    <hyperlink r:id="rId141" ref="C142"/>
+    <hyperlink r:id="rId142" ref="C143"/>
+    <hyperlink r:id="rId143" ref="C144"/>
+    <hyperlink r:id="rId144" ref="C145"/>
+    <hyperlink r:id="rId145" ref="C146"/>
+    <hyperlink r:id="rId146" ref="C147"/>
+    <hyperlink r:id="rId147" ref="C148"/>
+    <hyperlink r:id="rId148" ref="C149"/>
+    <hyperlink r:id="rId149" ref="C150"/>
+    <hyperlink r:id="rId150" ref="C151"/>
+    <hyperlink r:id="rId151" ref="C152"/>
+    <hyperlink r:id="rId152" ref="C153"/>
+    <hyperlink r:id="rId153" ref="C154"/>
+    <hyperlink r:id="rId154" ref="C155"/>
+    <hyperlink r:id="rId155" ref="C156"/>
   </hyperlinks>
-  <drawing r:id="rId132"/>
+  <drawing r:id="rId156"/>
   <tableParts count="1">
-    <tablePart r:id="rId134"/>
+    <tablePart r:id="rId158"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to skip button not finished yet
</commit_message>
<xml_diff>
--- a/src/Music.xlsx
+++ b/src/Music.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="431">
   <si>
     <t>Song Name</t>
   </si>
@@ -448,6 +448,9 @@
     <t>Disco Lines</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=sM9VJebg7bg</t>
+  </si>
+  <si>
     <t xml:space="preserve">disco boy </t>
   </si>
   <si>
@@ -475,12 +478,18 @@
     <t>Disco Lines &amp; John Summit</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=w6XFxc-XzRE</t>
+  </si>
+  <si>
     <t xml:space="preserve">fuck it up mike sherm </t>
   </si>
   <si>
     <t>Disco Lines &amp; Sidepiece</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=XtpQfeCWzqE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fuerteventura </t>
   </si>
   <si>
@@ -667,6 +676,9 @@
     <t>Gaslight</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=HxWrgmCJPjQ</t>
+  </si>
+  <si>
     <t xml:space="preserve">bla bla </t>
   </si>
   <si>
@@ -712,7 +724,7 @@
     <t>https://www.youtube.com/watch?v=S7XDsNraku4</t>
   </si>
   <si>
-    <t>wacka floca flame</t>
+    <t>Wacka Floca Flame</t>
   </si>
   <si>
     <t xml:space="preserve">grove st party </t>
@@ -931,7 +943,7 @@
     <t>The less I know the better</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=8jKT_kr-7eU</t>
+    <t>https://www.youtube.com/watch?v=-prcy6bqxCI</t>
   </si>
   <si>
     <t>Dress Code</t>
@@ -1223,13 +1235,82 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=ABAlIBtd_Ew</t>
+  </si>
+  <si>
+    <t>divine</t>
+  </si>
+  <si>
+    <t>blair muir</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=l2nINkFH7TY</t>
+  </si>
+  <si>
+    <t>morgan seatree</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=c_hXZadfCqc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it feeels so good </t>
+  </si>
+  <si>
+    <t>hugel and matt sassari</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LaVu0BjkzD8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">angel of mine </t>
+  </si>
+  <si>
+    <t>tobiahs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=YsYzfmJy8kw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nokia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">drake </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rQbyl-p4l_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goodf lies </t>
+  </si>
+  <si>
+    <t>overmono</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2KnbdLd_fVQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">salute </t>
+  </si>
+  <si>
+    <t>heaven in your arms</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=YYCic8pBTlo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nun major </t>
+  </si>
+  <si>
+    <t xml:space="preserve">disco lines </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1m7R1CY7K8M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1297,7 +1378,17 @@
     </font>
     <font>
       <u/>
-      <color rgb="FF434343"/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
   </fonts>
@@ -1483,7 +1574,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1541,13 +1632,16 @@
     <xf borderId="8" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1555,9 +1649,6 @@
     </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1574,13 +1665,19 @@
     <xf borderId="5" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="8" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1644,7 +1741,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D156" displayName="Music" name="Music" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:D164" displayName="Music" name="Music" id="1">
   <tableColumns count="4">
     <tableColumn name="Song Name" id="1"/>
     <tableColumn name="Artist" id="2"/>
@@ -2337,7 +2434,7 @@
       <c r="B34" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="19" t="s">
         <v>88</v>
       </c>
       <c r="D34" s="15" t="s">
@@ -2345,16 +2442,16 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="23" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2373,7 +2470,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="24" t="s">
         <v>94</v>
       </c>
       <c r="B37" s="9" t="s">
@@ -2533,7 +2630,7 @@
       <c r="B48" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="19" t="s">
         <v>120</v>
       </c>
       <c r="D48" s="15" t="s">
@@ -2569,16 +2666,16 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="D51" s="22" t="s">
+      <c r="D51" s="23" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2643,8 +2740,8 @@
       <c r="B56" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="17" t="s">
-        <v>88</v>
+      <c r="C56" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>7</v>
@@ -2652,13 +2749,13 @@
     </row>
     <row r="57">
       <c r="A57" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D57" s="11" t="s">
         <v>7</v>
@@ -2666,13 +2763,13 @@
     </row>
     <row r="58">
       <c r="A58" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D58" s="15" t="s">
         <v>7</v>
@@ -2680,13 +2777,13 @@
     </row>
     <row r="59">
       <c r="A59" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D59" s="11" t="s">
         <v>7</v>
@@ -2694,13 +2791,13 @@
     </row>
     <row r="60">
       <c r="A60" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>88</v>
+        <v>154</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>155</v>
       </c>
       <c r="D60" s="15" t="s">
         <v>7</v>
@@ -2708,13 +2805,13 @@
     </row>
     <row r="61">
       <c r="A61" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C61" s="18" t="s">
-        <v>88</v>
+        <v>157</v>
+      </c>
+      <c r="C61" s="28" t="s">
+        <v>158</v>
       </c>
       <c r="D61" s="11" t="s">
         <v>7</v>
@@ -2722,13 +2819,13 @@
     </row>
     <row r="62">
       <c r="A62" s="12" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D62" s="15" t="s">
         <v>7</v>
@@ -2736,13 +2833,13 @@
     </row>
     <row r="63">
       <c r="A63" s="8" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D63" s="11" t="s">
         <v>7</v>
@@ -2750,13 +2847,13 @@
     </row>
     <row r="64">
       <c r="A64" s="12" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>7</v>
@@ -2764,13 +2861,13 @@
     </row>
     <row r="65">
       <c r="A65" s="8" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D65" s="11" t="s">
         <v>7</v>
@@ -2778,55 +2875,55 @@
     </row>
     <row r="66">
       <c r="A66" s="4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="B67" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="C67" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="D67" s="22" t="s">
+      <c r="A67" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D67" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="12" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="8" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D69" s="11" t="s">
         <v>7</v>
@@ -2834,13 +2931,13 @@
     </row>
     <row r="70">
       <c r="A70" s="12" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D70" s="15" t="s">
         <v>7</v>
@@ -2848,13 +2945,13 @@
     </row>
     <row r="71">
       <c r="A71" s="8" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D71" s="11" t="s">
         <v>7</v>
@@ -2862,13 +2959,13 @@
     </row>
     <row r="72">
       <c r="A72" s="12" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D72" s="15" t="s">
         <v>7</v>
@@ -2876,13 +2973,13 @@
     </row>
     <row r="73">
       <c r="A73" s="8" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D73" s="11" t="s">
         <v>7</v>
@@ -2890,13 +2987,13 @@
     </row>
     <row r="74">
       <c r="A74" s="12" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D74" s="15" t="s">
         <v>7</v>
@@ -2904,13 +3001,13 @@
     </row>
     <row r="75">
       <c r="A75" s="8" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D75" s="11" t="s">
         <v>7</v>
@@ -2918,41 +3015,41 @@
     </row>
     <row r="76">
       <c r="A76" s="12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D76" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="B77" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="C77" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="D77" s="22" t="s">
+      <c r="A77" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D77" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="12" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D78" s="15" t="s">
         <v>7</v>
@@ -2960,13 +3057,13 @@
     </row>
     <row r="79">
       <c r="A79" s="8" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D79" s="11" t="s">
         <v>18</v>
@@ -2974,13 +3071,13 @@
     </row>
     <row r="80">
       <c r="A80" s="12" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D80" s="15" t="s">
         <v>7</v>
@@ -2988,13 +3085,13 @@
     </row>
     <row r="81">
       <c r="A81" s="8" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D81" s="11" t="s">
         <v>7</v>
@@ -3002,41 +3099,41 @@
     </row>
     <row r="82">
       <c r="A82" s="12" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D82" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="B83" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="C83" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D83" s="22" t="s">
+      <c r="A83" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="C83" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D83" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>7</v>
@@ -3044,13 +3141,13 @@
     </row>
     <row r="85">
       <c r="A85" s="8" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D85" s="11" t="s">
         <v>7</v>
@@ -3058,13 +3155,13 @@
     </row>
     <row r="86">
       <c r="A86" s="12" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C86" s="17" t="s">
-        <v>88</v>
+        <v>220</v>
+      </c>
+      <c r="C86" s="19" t="s">
+        <v>221</v>
       </c>
       <c r="D86" s="15" t="s">
         <v>7</v>
@@ -3072,13 +3169,13 @@
     </row>
     <row r="87">
       <c r="A87" s="8" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D87" s="11" t="s">
         <v>142</v>
@@ -3086,13 +3183,13 @@
     </row>
     <row r="88">
       <c r="A88" s="12" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D88" s="15" t="s">
         <v>18</v>
@@ -3100,13 +3197,13 @@
     </row>
     <row r="89">
       <c r="A89" s="8" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D89" s="11" t="s">
         <v>18</v>
@@ -3114,13 +3211,13 @@
     </row>
     <row r="90">
       <c r="A90" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B90" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="B90" s="13" t="s">
-        <v>222</v>
-      </c>
       <c r="C90" s="17" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D90" s="15" t="s">
         <v>18</v>
@@ -3128,13 +3225,13 @@
     </row>
     <row r="91">
       <c r="A91" s="8" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D91" s="11" t="s">
         <v>18</v>
@@ -3142,13 +3239,13 @@
     </row>
     <row r="92">
       <c r="A92" s="12" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>7</v>
@@ -3156,13 +3253,13 @@
     </row>
     <row r="93">
       <c r="A93" s="8" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="C93" s="18" t="s">
-        <v>235</v>
+        <v>238</v>
+      </c>
+      <c r="C93" s="28" t="s">
+        <v>239</v>
       </c>
       <c r="D93" s="11" t="s">
         <v>7</v>
@@ -3170,27 +3267,27 @@
     </row>
     <row r="94">
       <c r="A94" s="12" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="8" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D95" s="11" t="s">
         <v>7</v>
@@ -3198,13 +3295,13 @@
     </row>
     <row r="96">
       <c r="A96" s="12" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="D96" s="15" t="s">
         <v>96</v>
@@ -3212,13 +3309,13 @@
     </row>
     <row r="97">
       <c r="A97" s="8" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D97" s="11" t="s">
         <v>7</v>
@@ -3226,13 +3323,13 @@
     </row>
     <row r="98">
       <c r="A98" s="12" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D98" s="15" t="s">
         <v>7</v>
@@ -3240,13 +3337,13 @@
     </row>
     <row r="99">
       <c r="A99" s="8" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C99" s="28" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D99" s="11" t="s">
         <v>7</v>
@@ -3254,13 +3351,13 @@
     </row>
     <row r="100">
       <c r="A100" s="12" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D100" s="15" t="s">
         <v>7</v>
@@ -3268,13 +3365,13 @@
     </row>
     <row r="101">
       <c r="A101" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B101" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="B101" s="9" t="s">
-        <v>253</v>
-      </c>
       <c r="C101" s="10" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D101" s="11" t="s">
         <v>7</v>
@@ -3282,13 +3379,13 @@
     </row>
     <row r="102">
       <c r="A102" s="12" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D102" s="15" t="s">
         <v>7</v>
@@ -3296,13 +3393,13 @@
     </row>
     <row r="103">
       <c r="A103" s="8" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C103" s="18" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D103" s="11" t="s">
         <v>7</v>
@@ -3310,13 +3407,13 @@
     </row>
     <row r="104">
       <c r="A104" s="4" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D104" s="7" t="s">
         <v>7</v>
@@ -3324,13 +3421,13 @@
     </row>
     <row r="105">
       <c r="A105" s="8" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="D105" s="11" t="s">
         <v>7</v>
@@ -3338,97 +3435,97 @@
     </row>
     <row r="106">
       <c r="A106" s="12" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D106" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="19" t="s">
-        <v>269</v>
-      </c>
-      <c r="B107" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="C107" s="21" t="s">
-        <v>270</v>
-      </c>
-      <c r="D107" s="22" t="s">
+      <c r="A107" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="C107" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="D107" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="12" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C108" s="29" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="D108" s="15" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="B109" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="C109" s="21" t="s">
-        <v>275</v>
-      </c>
-      <c r="D109" s="22" t="s">
+      <c r="A109" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="C109" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="D109" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="12" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C110" s="29" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D110" s="15" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="8" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="12" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D112" s="15" t="s">
         <v>7</v>
@@ -3436,13 +3533,13 @@
     </row>
     <row r="113">
       <c r="A113" s="8" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D113" s="11" t="s">
         <v>7</v>
@@ -3450,67 +3547,67 @@
     </row>
     <row r="114">
       <c r="A114" s="12" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D114" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="B115" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="C115" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="D115" s="22"/>
+      <c r="A115" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="B115" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="C115" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="D115" s="23"/>
     </row>
     <row r="116">
       <c r="A116" s="12" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D116" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="19" t="s">
-        <v>296</v>
-      </c>
-      <c r="B117" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="C117" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="D117" s="22" t="s">
+      <c r="A117" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="B117" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="C117" s="22" t="s">
+        <v>302</v>
+      </c>
+      <c r="D117" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="12" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C118" s="17" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="D118" s="15" t="s">
         <v>7</v>
@@ -3518,13 +3615,13 @@
     </row>
     <row r="119">
       <c r="A119" s="8" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="D119" s="11" t="s">
         <v>7</v>
@@ -3532,69 +3629,69 @@
     </row>
     <row r="120">
       <c r="A120" s="12" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C120" s="17" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D120" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="19" t="s">
+      <c r="A121" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="B121" s="21" t="s">
         <v>307</v>
       </c>
-      <c r="B121" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="C121" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="D121" s="22" t="s">
+      <c r="C121" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="D121" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="4" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D122" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="19" t="s">
-        <v>311</v>
-      </c>
-      <c r="B123" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="C123" s="21" t="s">
-        <v>312</v>
-      </c>
-      <c r="D123" s="22" t="s">
+      <c r="A123" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="B123" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="C123" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="D123" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="12" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D124" s="15" t="s">
         <v>7</v>
@@ -3602,13 +3699,13 @@
     </row>
     <row r="125">
       <c r="A125" s="8" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C125" s="18" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="D125" s="11" t="s">
         <v>7</v>
@@ -3616,27 +3713,27 @@
     </row>
     <row r="126">
       <c r="A126" s="4" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D126" s="7" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="8" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D127" s="11" t="s">
         <v>7</v>
@@ -3644,13 +3741,13 @@
     </row>
     <row r="128">
       <c r="A128" s="12" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D128" s="15" t="s">
         <v>7</v>
@@ -3658,27 +3755,27 @@
     </row>
     <row r="129">
       <c r="A129" s="8" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="C129" s="10" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="D129" s="11" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="4" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D130" s="7" t="s">
         <v>7</v>
@@ -3686,13 +3783,13 @@
     </row>
     <row r="131">
       <c r="A131" s="8" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C131" s="10" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="D131" s="11" t="s">
         <v>96</v>
@@ -3700,13 +3797,13 @@
     </row>
     <row r="132">
       <c r="A132" s="4" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="D132" s="7" t="s">
         <v>7</v>
@@ -3714,13 +3811,13 @@
     </row>
     <row r="133">
       <c r="A133" s="8" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="C133" s="18" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="D133" s="11" t="s">
         <v>7</v>
@@ -3728,13 +3825,13 @@
     </row>
     <row r="134">
       <c r="A134" s="12" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C134" s="17" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="D134" s="15" t="s">
         <v>142</v>
@@ -3742,13 +3839,13 @@
     </row>
     <row r="135">
       <c r="A135" s="8" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D135" s="11" t="s">
         <v>7</v>
@@ -3756,13 +3853,13 @@
     </row>
     <row r="136">
       <c r="A136" s="12" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C136" s="17" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="D136" s="15" t="s">
         <v>7</v>
@@ -3770,13 +3867,13 @@
     </row>
     <row r="137">
       <c r="A137" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B137" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="B137" s="9" t="s">
-        <v>346</v>
-      </c>
       <c r="C137" s="18" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="D137" s="11" t="s">
         <v>7</v>
@@ -3784,13 +3881,13 @@
     </row>
     <row r="138">
       <c r="A138" s="12" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C138" s="17" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="D138" s="15" t="s">
         <v>7</v>
@@ -3798,13 +3895,13 @@
     </row>
     <row r="139">
       <c r="A139" s="8" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="D139" s="11" t="s">
         <v>96</v>
@@ -3812,13 +3909,13 @@
     </row>
     <row r="140">
       <c r="A140" s="12" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="C140" s="14" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="D140" s="15" t="s">
         <v>7</v>
@@ -3826,13 +3923,13 @@
     </row>
     <row r="141">
       <c r="A141" s="8" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="D141" s="11" t="s">
         <v>18</v>
@@ -3840,13 +3937,13 @@
     </row>
     <row r="142">
       <c r="A142" s="12" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="C142" s="17" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="D142" s="15" t="s">
         <v>7</v>
@@ -3854,13 +3951,13 @@
     </row>
     <row r="143">
       <c r="A143" s="8" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="C143" s="18" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="D143" s="11" t="s">
         <v>7</v>
@@ -3868,13 +3965,13 @@
     </row>
     <row r="144">
       <c r="A144" s="12" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C144" s="17" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D144" s="15" t="s">
         <v>96</v>
@@ -3882,13 +3979,13 @@
     </row>
     <row r="145">
       <c r="A145" s="8" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="C145" s="18" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="D145" s="11" t="s">
         <v>142</v>
@@ -3896,13 +3993,13 @@
     </row>
     <row r="146">
       <c r="A146" s="12" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C146" s="14" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D146" s="15" t="s">
         <v>7</v>
@@ -3910,13 +4007,13 @@
     </row>
     <row r="147">
       <c r="A147" s="8" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C147" s="10" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="D147" s="11" t="s">
         <v>7</v>
@@ -3924,13 +4021,13 @@
     </row>
     <row r="148">
       <c r="A148" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="B148" s="13" t="s">
         <v>380</v>
       </c>
-      <c r="B148" s="13" t="s">
-        <v>376</v>
-      </c>
       <c r="C148" s="14" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="D148" s="15" t="s">
         <v>7</v>
@@ -3938,13 +4035,13 @@
     </row>
     <row r="149">
       <c r="A149" s="8" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="C149" s="10" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="D149" s="11" t="s">
         <v>7</v>
@@ -3952,13 +4049,13 @@
     </row>
     <row r="150">
       <c r="A150" s="12" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="C150" s="14" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D150" s="15" t="s">
         <v>7</v>
@@ -3966,13 +4063,13 @@
     </row>
     <row r="151">
       <c r="A151" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="B151" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="B151" s="9" t="s">
-        <v>383</v>
-      </c>
       <c r="C151" s="18" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="D151" s="11" t="s">
         <v>7</v>
@@ -3980,13 +4077,13 @@
     </row>
     <row r="152">
       <c r="A152" s="12" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="D152" s="15" t="s">
         <v>7</v>
@@ -3994,13 +4091,13 @@
     </row>
     <row r="153">
       <c r="A153" s="8" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="D153" s="11" t="s">
         <v>7</v>
@@ -4008,49 +4105,161 @@
     </row>
     <row r="154">
       <c r="A154" s="4" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B154" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="D154" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="20" t="s">
+        <v>402</v>
+      </c>
+      <c r="B155" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="C155" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="D155" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="D156" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="20" t="s">
+        <v>408</v>
+      </c>
+      <c r="B157" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="C157" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="D157" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="C154" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="D154" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" s="19" t="s">
-        <v>398</v>
-      </c>
-      <c r="B155" s="20" t="s">
-        <v>399</v>
-      </c>
-      <c r="C155" s="21" t="s">
-        <v>400</v>
-      </c>
-      <c r="D155" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="30" t="s">
-        <v>401</v>
-      </c>
-      <c r="B156" s="31" t="s">
-        <v>402</v>
-      </c>
-      <c r="C156" s="32" t="s">
-        <v>403</v>
-      </c>
-      <c r="D156" s="33" t="s">
-        <v>7</v>
+      <c r="B158" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C158" s="31" t="s">
+        <v>412</v>
+      </c>
+      <c r="D158" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="B159" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="C159" s="30" t="s">
+        <v>415</v>
+      </c>
+      <c r="D159" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="C160" s="31" t="s">
+        <v>418</v>
+      </c>
+      <c r="D160" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="20" t="s">
+        <v>419</v>
+      </c>
+      <c r="B161" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="C161" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="D161" s="23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="C162" s="31" t="s">
+        <v>424</v>
+      </c>
+      <c r="D162" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="B163" s="21" t="s">
+        <v>426</v>
+      </c>
+      <c r="C163" s="30" t="s">
+        <v>427</v>
+      </c>
+      <c r="D163" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="32" t="s">
+        <v>428</v>
+      </c>
+      <c r="B164" s="33" t="s">
+        <v>429</v>
+      </c>
+      <c r="C164" s="34" t="s">
+        <v>430</v>
+      </c>
+      <c r="D164" s="35" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="D2:D156">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="D2:D164">
       <formula1>"LATIN HOUSE,SUNSET HOUSE,TECH HOUSE,HOUSE,DJTOOLS,ELECTRO POP,AFRO HOUSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4210,10 +4419,18 @@
     <hyperlink r:id="rId153" ref="C154"/>
     <hyperlink r:id="rId154" ref="C155"/>
     <hyperlink r:id="rId155" ref="C156"/>
+    <hyperlink r:id="rId156" ref="C157"/>
+    <hyperlink r:id="rId157" ref="C158"/>
+    <hyperlink r:id="rId158" ref="C159"/>
+    <hyperlink r:id="rId159" ref="C160"/>
+    <hyperlink r:id="rId160" ref="C161"/>
+    <hyperlink r:id="rId161" ref="C162"/>
+    <hyperlink r:id="rId162" ref="C163"/>
+    <hyperlink r:id="rId163" ref="C164"/>
   </hyperlinks>
-  <drawing r:id="rId156"/>
+  <drawing r:id="rId164"/>
   <tableParts count="1">
-    <tablePart r:id="rId158"/>
+    <tablePart r:id="rId166"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>